<commit_message>
Fix small bugs with polls, add the decorator to avoid cheating
</commit_message>
<xml_diff>
--- a/data/Routesetting.xlsx
+++ b/data/Routesetting.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="PATTERN" sheetId="1" state="visible" r:id="rId1"/>
@@ -789,11 +789,11 @@
   </sheetPr>
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O11" activeCellId="1" sqref="C4:K4 O11"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.90234375" defaultRowHeight="15.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="28">
       <c r="A1" s="29" t="n"/>
@@ -2710,11 +2710,11 @@
   </sheetPr>
   <dimension ref="A1:BM59"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4:K4"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.90234375" defaultRowHeight="15.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="9.51" customWidth="1" style="60" min="3" max="14"/>
     <col width="10.12" customWidth="1" style="60" min="15" max="15"/>
@@ -2972,7 +2972,6 @@
       <c r="K4" s="61" t="n">
         <v>44712</v>
       </c>
-      <c r="L4" s="60" t="n"/>
       <c r="M4" s="32" t="n"/>
       <c r="N4" s="32" t="n"/>
       <c r="O4" s="30" t="n"/>
@@ -4896,11 +4895,11 @@
   </sheetPr>
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.90234375" defaultRowHeight="15.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="28">
       <c r="A1" s="29" t="n"/>
@@ -5144,7 +5143,9 @@
       <c r="C6" s="34" t="n"/>
       <c r="D6" s="35" t="n"/>
       <c r="E6" s="35" t="n"/>
-      <c r="F6" s="35" t="n"/>
+      <c r="F6" s="35" t="n">
+        <v>1</v>
+      </c>
       <c r="G6" s="35" t="n"/>
       <c r="H6" s="35" t="n"/>
       <c r="I6" s="35" t="n">
@@ -5181,7 +5182,9 @@
       <c r="C7" s="40" t="n"/>
       <c r="D7" s="41" t="n"/>
       <c r="E7" s="41" t="n"/>
-      <c r="F7" s="41" t="n"/>
+      <c r="F7" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" s="41" t="n"/>
       <c r="H7" s="41" t="n"/>
       <c r="I7" s="41" t="n">
@@ -5223,7 +5226,9 @@
       <c r="C8" s="40" t="n"/>
       <c r="D8" s="41" t="n"/>
       <c r="E8" s="41" t="n"/>
-      <c r="F8" s="41" t="n"/>
+      <c r="F8" s="41" t="n">
+        <v>1</v>
+      </c>
       <c r="G8" s="41" t="n"/>
       <c r="H8" s="41" t="n"/>
       <c r="I8" s="41" t="n">
@@ -5261,7 +5266,9 @@
       <c r="C9" s="40" t="n"/>
       <c r="D9" s="41" t="n"/>
       <c r="E9" s="41" t="n"/>
-      <c r="F9" s="41" t="n"/>
+      <c r="F9" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="G9" s="41" t="n"/>
       <c r="H9" s="41" t="n"/>
       <c r="I9" s="41" t="n">
@@ -5301,7 +5308,9 @@
       <c r="C10" s="40" t="n"/>
       <c r="D10" s="41" t="n"/>
       <c r="E10" s="41" t="n"/>
-      <c r="F10" s="41" t="n"/>
+      <c r="F10" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="G10" s="41" t="n"/>
       <c r="H10" s="41" t="n"/>
       <c r="I10" s="41" t="n">
@@ -5567,7 +5576,11 @@
       <c r="T17" s="29" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="28">
-      <c r="A18" s="33" t="n"/>
+      <c r="A18" s="33" t="inlineStr">
+        <is>
+          <t>@rutserser</t>
+        </is>
+      </c>
       <c r="B18" s="33" t="n">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
the richest func correct
</commit_message>
<xml_diff>
--- a/data/Routesetting.xlsx
+++ b/data/Routesetting.xlsx
@@ -1414,7 +1414,11 @@
       <c r="T17" s="29" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="28">
-      <c r="A18" s="33" t="n"/>
+      <c r="A18" s="33" t="inlineStr">
+        <is>
+          <t>@kraslavchik_pl</t>
+        </is>
+      </c>
       <c r="B18" s="33" t="n">
         <v>5</v>
       </c>
@@ -5578,7 +5582,7 @@
     <row r="18" ht="15.75" customHeight="1" s="28">
       <c r="A18" s="33" t="inlineStr">
         <is>
-          <t>@rutserser</t>
+          <t>@kraslavchik_pl</t>
         </is>
       </c>
       <c r="B18" s="33" t="n">
@@ -5587,7 +5591,9 @@
       <c r="C18" s="40" t="n"/>
       <c r="D18" s="41" t="n"/>
       <c r="E18" s="41" t="n"/>
-      <c r="F18" s="41" t="n"/>
+      <c r="F18" s="41" t="n">
+        <v>4</v>
+      </c>
       <c r="G18" s="41" t="n"/>
       <c r="H18" s="41" t="n"/>
       <c r="I18" s="41" t="n"/>
@@ -5622,7 +5628,9 @@
       <c r="C19" s="40" t="n"/>
       <c r="D19" s="41" t="n"/>
       <c r="E19" s="41" t="n"/>
-      <c r="F19" s="41" t="n"/>
+      <c r="F19" s="41" t="n">
+        <v>3</v>
+      </c>
       <c r="G19" s="41" t="n"/>
       <c r="H19" s="41" t="n"/>
       <c r="I19" s="41" t="n"/>
@@ -5654,7 +5662,9 @@
       <c r="C20" s="40" t="n"/>
       <c r="D20" s="41" t="n"/>
       <c r="E20" s="41" t="n"/>
-      <c r="F20" s="41" t="n"/>
+      <c r="F20" s="41" t="n">
+        <v>4</v>
+      </c>
       <c r="G20" s="41" t="n"/>
       <c r="H20" s="41" t="n"/>
       <c r="I20" s="41" t="n"/>
@@ -5686,7 +5696,9 @@
       <c r="C21" s="40" t="n"/>
       <c r="D21" s="41" t="n"/>
       <c r="E21" s="41" t="n"/>
-      <c r="F21" s="41" t="n"/>
+      <c r="F21" s="41" t="n">
+        <v>3</v>
+      </c>
       <c r="G21" s="41" t="n"/>
       <c r="H21" s="41" t="n"/>
       <c r="I21" s="41" t="n"/>
@@ -5718,7 +5730,9 @@
       <c r="C22" s="40" t="n"/>
       <c r="D22" s="41" t="n"/>
       <c r="E22" s="41" t="n"/>
-      <c r="F22" s="41" t="n"/>
+      <c r="F22" s="41" t="n">
+        <v>3</v>
+      </c>
       <c r="G22" s="41" t="n"/>
       <c r="H22" s="41" t="n"/>
       <c r="I22" s="41" t="n"/>

</xml_diff>